<commit_message>
added new fields for customer and enhance upload feature
</commit_message>
<xml_diff>
--- a/template/Customer_Template.xlsx
+++ b/template/Customer_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/speedjin/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jihbi\xampp\htdocs\synctronix\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6391B0D7-D41A-444C-B599-2454C517CB70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F099BC7A-24F0-42B0-9CAC-668E3D7B2BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{9341FD95-CFC6-421C-9B6B-E00C8B5A4387}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9341FD95-CFC6-421C-9B6B-E00C8B5A4387}"/>
   </bookViews>
   <sheets>
     <sheet name="customermaster" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Code</t>
   </si>
@@ -40,13 +40,22 @@
     <t>Addr3</t>
   </si>
   <si>
-    <t>Addr4</t>
-  </si>
-  <si>
     <t>Tel</t>
   </si>
   <si>
     <t>Fax</t>
+  </si>
+  <si>
+    <t>New Reg No</t>
+  </si>
+  <si>
+    <t>Contact Name</t>
+  </si>
+  <si>
+    <t>Tin No</t>
+  </si>
+  <si>
+    <t>IC No</t>
   </si>
 </sst>
 </file>
@@ -398,26 +407,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E7AE52E-5E3F-4816-BCAD-C318F36103B6}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="7" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" customWidth="1"/>
+    <col min="14" max="14" width="6.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -428,22 +440,31 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>